<commit_message>
data lessen aangepast + nieuwe pagina verdieping
</commit_message>
<xml_diff>
--- a/flyers/Grimbergen_2018-2019.xlsx
+++ b/flyers/Grimbergen_2018-2019.xlsx
@@ -698,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:Q135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I78" activeCellId="0" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3479,14 +3479,14 @@
       <c r="H78" s="26" t="n">
         <v>8</v>
       </c>
-      <c r="I78" s="31" t="s">
-        <v>14</v>
+      <c r="I78" s="30" t="s">
+        <v>15</v>
       </c>
       <c r="J78" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K78" s="31" t="s">
-        <v>14</v>
+      <c r="K78" s="30" t="s">
+        <v>15</v>
       </c>
       <c r="L78" s="24"/>
       <c r="M78" s="27" t="s">
@@ -3744,14 +3744,14 @@
       <c r="H85" s="26" t="n">
         <v>15</v>
       </c>
-      <c r="I85" s="29" t="s">
-        <v>15</v>
+      <c r="I85" s="31" t="s">
+        <v>14</v>
       </c>
       <c r="J85" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K85" s="30" t="s">
-        <v>15</v>
+      <c r="K85" s="31" t="s">
+        <v>14</v>
       </c>
       <c r="L85" s="24"/>
       <c r="M85" s="27" t="s">

</xml_diff>

<commit_message>
nieuwe stage + wisselen data
</commit_message>
<xml_diff>
--- a/flyers/Grimbergen_2018-2019.xlsx
+++ b/flyers/Grimbergen_2018-2019.xlsx
@@ -698,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:Q135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I78" activeCellId="0" sqref="I78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="B69" colorId="64" zoomScale="75" zoomScaleNormal="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D84" activeCellId="0" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3336,8 +3336,8 @@
         <v>4</v>
       </c>
       <c r="I74" s="26"/>
-      <c r="J74" s="31" t="s">
-        <v>14</v>
+      <c r="J74" s="30" t="s">
+        <v>15</v>
       </c>
       <c r="K74" s="30" t="s">
         <v>15</v>
@@ -3696,8 +3696,8 @@
         <v>14</v>
       </c>
       <c r="C84" s="34"/>
-      <c r="D84" s="30" t="s">
-        <v>15</v>
+      <c r="D84" s="31" t="s">
+        <v>14</v>
       </c>
       <c r="E84" s="30" t="s">
         <v>15</v>
@@ -3975,8 +3975,8 @@
         <v>21</v>
       </c>
       <c r="C91" s="26"/>
-      <c r="D91" s="31" t="s">
-        <v>14</v>
+      <c r="D91" s="30" t="s">
+        <v>15</v>
       </c>
       <c r="E91" s="30" t="s">
         <v>15</v>
@@ -4246,8 +4246,8 @@
         <v>28</v>
       </c>
       <c r="C98" s="34"/>
-      <c r="D98" s="30" t="s">
-        <v>15</v>
+      <c r="D98" s="31" t="s">
+        <v>14</v>
       </c>
       <c r="E98" s="30" t="s">
         <v>15</v>

</xml_diff>